<commit_message>
order sent to jlcpcb
</commit_message>
<xml_diff>
--- a/Kicad_Project/MANUFACTURE/MP2_DFN_BOM.xlsx
+++ b/Kicad_Project/MANUFACTURE/MP2_DFN_BOM.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10107"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/owhite/kicad/MP2-DFN/Kicad_Project/MANUFACTURE/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C7AC2096-0D96-5A4E-99EA-6E328E6AB2E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{E4FAF919-BABB-EE4D-BA9D-DEDD18BEA6A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20380" yWindow="5400" windowWidth="28040" windowHeight="17440"/>
+    <workbookView xWindow="42660" yWindow="5340" windowWidth="28040" windowHeight="17440"/>
   </bookViews>
   <sheets>
     <sheet name="MP2_DFN" sheetId="1" r:id="rId1"/>
@@ -412,7 +412,7 @@
     <t>C531304</t>
   </si>
   <si>
-    <t>NCP5183 / TF2190-TAH</t>
+    <t>TF2190-TAH</t>
   </si>
   <si>
     <t>U1,U2,U3</t>
@@ -1869,6 +1869,6 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>